<commit_message>
New: Custom Number Range for Processing; Improve: Better handling of column names; New: Puts state in output-file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-assessment-settings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8673C8C3-BF6B-4258-BA2F-7A236C4FA375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE745D2D-19CF-4CB5-9109-F6DEC54A6BA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>How many minutes later than the test closing is the course closing?</t>
+  </si>
+  <si>
+    <t>CustomTransactionNumbers</t>
+  </si>
+  <si>
+    <t>Empty, if all rows of Input File shall be processed. A semicolon separated list of Excel Row Numbers (3;6;20) or a hypen separated range of Excel Row Numbers (3-20), if only these Excel Rows shall be processed.</t>
+  </si>
+  <si>
+    <t>2-8</t>
+  </si>
+  <si>
+    <t>OutputDataFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\</t>
+  </si>
+  <si>
+    <t>Path, where the Output Excel Workbooks are saved</t>
   </si>
 </sst>
 </file>
@@ -272,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -283,6 +301,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -597,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -667,90 +686,110 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" ht="45">
+      <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="30">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="30">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>120</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1730,6 +1769,8 @@
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve: Switch Password field empty before entering; Destroy: no dynamic opening date/time
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-assessment-settings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE745D2D-19CF-4CB5-9109-F6DEC54A6BA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DED3A6F-C42A-4A0D-A104-13F872D5EC63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,9 +229,6 @@
     <t>Empty, if all rows of Input File shall be processed. A semicolon separated list of Excel Row Numbers (3;6;20) or a hypen separated range of Excel Row Numbers (3-20), if only these Excel Rows shall be processed.</t>
   </si>
   <si>
-    <t>2-8</t>
-  </si>
-  <si>
     <t>OutputDataFilePath</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Path, where the Output Excel Workbooks are saved</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -691,7 +691,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>67</v>
@@ -699,13 +699,13 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>